<commit_message>
Update, Login System with GUI
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -322,7 +322,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -354,6 +354,66 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Freesia</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Freesia1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>a_guy</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>hhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>dd</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ff</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>iii</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>iii</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>seemore</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>butts</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>